<commit_message>
Finale Überabreitung des Statusberichts 2
</commit_message>
<xml_diff>
--- a/21-01-04_Statusbericht_2/20-11-20_Gantt_Chart.xlsx
+++ b/21-01-04_Statusbericht_2/20-11-20_Gantt_Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heiko\Documents\AAA_Studium\WiSe20\bachelorprojekt2020\20-11-23_Statusbericht\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heiko\Documents\AAA_Studium\WiSe20\bachelorprojekt2020\21-01-04_Statusbericht_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DE1F42-9F0B-42DD-A624-4014D09B8FE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8CCBD5-CBD2-4206-92C8-3467ECB3A12B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{905C64CD-B653-4290-BF74-D3CE989EBBEF}"/>
   </bookViews>
@@ -108,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +116,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +149,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,17 +168,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -187,16 +210,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>2420</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>24356</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>45983</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>663464</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>6569</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>367388</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -211,10 +234,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7459134" y="998483"/>
-          <a:ext cx="2185044" cy="831443"/>
-          <a:chOff x="7460495" y="998483"/>
-          <a:chExt cx="2185044" cy="817836"/>
+          <a:off x="4641180" y="1222601"/>
+          <a:ext cx="4836590" cy="2251223"/>
+          <a:chOff x="6146317" y="998483"/>
+          <a:chExt cx="3499222" cy="817836"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -235,10 +258,13 @@
           </a:xfrm>
           <a:prstGeom prst="wedgeRectCallout">
             <a:avLst>
-              <a:gd name="adj1" fmla="val -228225"/>
-              <a:gd name="adj2" fmla="val -6373"/>
+              <a:gd name="adj1" fmla="val -208462"/>
+              <a:gd name="adj2" fmla="val -36419"/>
             </a:avLst>
           </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
@@ -262,11 +288,11 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="de-DE" sz="1100"/>
+              <a:rPr lang="de-DE" sz="2000"/>
               <a:t>Telko mit Projektpartner hat</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+              <a:rPr lang="de-DE" sz="2000" baseline="0"/>
               <a:t> neue Anforderungen hervorgebracht</a:t>
             </a:r>
           </a:p>
@@ -285,14 +311,17 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm rot="15985021">
-            <a:off x="7753897" y="1449125"/>
-            <a:ext cx="71184" cy="657987"/>
+            <a:off x="7078731" y="306802"/>
+            <a:ext cx="136169" cy="2000997"/>
           </a:xfrm>
           <a:prstGeom prst="triangle">
             <a:avLst>
-              <a:gd name="adj" fmla="val 83374"/>
+              <a:gd name="adj" fmla="val 80605"/>
             </a:avLst>
           </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
@@ -348,8 +377,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12668249" y="585108"/>
-          <a:ext cx="439830" cy="9837964"/>
+          <a:off x="10915329" y="719579"/>
+          <a:ext cx="439830" cy="11208283"/>
           <a:chOff x="6721928" y="367393"/>
           <a:chExt cx="439830" cy="9837964"/>
         </a:xfrm>
@@ -446,16 +475,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>482724</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>116740</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>584777</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>489293</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>77326</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>578304</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>68035</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -470,8 +499,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17001795" y="5614026"/>
-          <a:ext cx="1530569" cy="831443"/>
+          <a:off x="16981384" y="6852275"/>
+          <a:ext cx="1748849" cy="1516117"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -479,6 +508,9 @@
             <a:gd name="adj2" fmla="val -6373"/>
           </a:avLst>
         </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -502,11 +534,11 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100"/>
+            <a:rPr lang="de-DE" sz="1800"/>
             <a:t>Corona-Bedingte</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:rPr lang="de-DE" sz="1800" baseline="0"/>
             <a:t> Zugangsbeschränkung zur Hochschule</a:t>
           </a:r>
         </a:p>
@@ -516,16 +548,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>708904</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>2373</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6404</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>715473</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>123871</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>232122</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -540,15 +572,18 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10451618" y="3918857"/>
-          <a:ext cx="1530569" cy="831443"/>
+          <a:off x="15320814" y="2964757"/>
+          <a:ext cx="1488010" cy="1256659"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -142879"/>
-            <a:gd name="adj2" fmla="val -16192"/>
+            <a:gd name="adj1" fmla="val -120286"/>
+            <a:gd name="adj2" fmla="val 122024"/>
           </a:avLst>
         </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -572,7 +607,7 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:rPr lang="de-DE" sz="2000" baseline="0"/>
             <a:t>Priorität wurde verschoben</a:t>
           </a:r>
         </a:p>
@@ -584,14 +619,14 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>28547</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>35116</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>163284</xdr:rowOff>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>122463</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -606,10 +641,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="13499618" y="1823357"/>
-          <a:ext cx="1530569" cy="3211284"/>
-          <a:chOff x="8114970" y="998483"/>
-          <a:chExt cx="1530569" cy="3158729"/>
+          <a:off x="11850753" y="1855373"/>
+          <a:ext cx="1504258" cy="4318266"/>
+          <a:chOff x="8114970" y="730794"/>
+          <a:chExt cx="1862846" cy="3587032"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -625,15 +660,18 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8114970" y="998483"/>
-            <a:ext cx="1530569" cy="817836"/>
+            <a:off x="8114970" y="730794"/>
+            <a:ext cx="1862846" cy="1084142"/>
           </a:xfrm>
           <a:prstGeom prst="wedgeRectCallout">
             <a:avLst>
-              <a:gd name="adj1" fmla="val -225558"/>
-              <a:gd name="adj2" fmla="val 157284"/>
+              <a:gd name="adj1" fmla="val -262779"/>
+              <a:gd name="adj2" fmla="val 120989"/>
             </a:avLst>
           </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
@@ -657,10 +695,10 @@
           <a:p>
             <a:pPr algn="l"/>
             <a:r>
-              <a:rPr lang="de-DE" sz="1100"/>
+              <a:rPr lang="de-DE" sz="2000"/>
               <a:t>Komplexität weitaus höher als erwartet</a:t>
             </a:r>
-            <a:endParaRPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:endParaRPr lang="de-DE" sz="2000" baseline="0"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -677,14 +715,17 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm rot="10800000" flipH="1">
-            <a:off x="8490225" y="1828018"/>
-            <a:ext cx="140484" cy="2329194"/>
+            <a:off x="8423035" y="1710234"/>
+            <a:ext cx="194206" cy="2607592"/>
           </a:xfrm>
           <a:prstGeom prst="triangle">
             <a:avLst>
               <a:gd name="adj" fmla="val 83374"/>
             </a:avLst>
           </a:prstGeom>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
         </xdr:spPr>
         <xdr:style>
           <a:lnRef idx="2">
@@ -1016,385 +1057,466 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D7FA78-90B6-4B5B-A677-AB96A65F19BC}">
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" style="2" customWidth="1"/>
-    <col min="27" max="27" width="26.5703125" style="2" customWidth="1"/>
+    <col min="2" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="1" customWidth="1"/>
+    <col min="8" max="13" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" style="1" customWidth="1"/>
+    <col min="15" max="26" width="8.7109375" customWidth="1"/>
+    <col min="27" max="27" width="28" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="A1" t="s">
+    <row r="1" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
-      <c r="A2" t="s">
+    <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
-      <c r="A4" t="s">
+    <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="G3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="AA3" s="14"/>
+    </row>
+    <row r="4" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="15">
         <v>44158</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="15">
         <v>43834</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AA4" s="15">
         <v>43920</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
-      <c r="A5" t="s">
+    <row r="5" spans="1:27" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="12">
         <v>44126</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="12">
         <v>44133</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="12">
         <v>44140</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="12">
         <v>44147</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="12">
         <v>44154</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="1">
+      <c r="G5" s="13"/>
+      <c r="H5" s="12">
         <v>44161</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="12">
         <v>44168</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="12">
         <v>44175</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="12">
         <v>44182</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="12">
         <v>44189</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="12">
         <v>44196</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="1">
+      <c r="N5" s="13"/>
+      <c r="O5" s="12">
         <v>44203</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="12">
         <v>44210</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="12">
         <v>44217</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="12">
         <v>44224</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="12">
         <v>44231</v>
       </c>
-      <c r="T5" s="1">
+      <c r="T5" s="12">
         <v>44238</v>
       </c>
-      <c r="U5" s="1">
+      <c r="U5" s="12">
         <v>44245</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="12">
         <v>44252</v>
       </c>
-      <c r="W5" s="1">
+      <c r="W5" s="12">
         <v>44259</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5" s="12">
         <v>44266</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Y5" s="12">
         <v>44273</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="Z5" s="12">
         <v>44280</v>
       </c>
-    </row>
-    <row r="7" spans="1:27">
-      <c r="A7" t="s">
+      <c r="AA5" s="16"/>
+    </row>
+    <row r="6" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:27" ht="3.95" customHeight="1">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="10" spans="1:27">
-      <c r="A10" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+    </row>
+    <row r="10" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:27" ht="3.95" customHeight="1">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="13" spans="1:27">
-      <c r="A13" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+    </row>
+    <row r="13" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:27" ht="3.95" customHeight="1">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="A16" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:27" ht="3.95" customHeight="1">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="19" spans="1:27">
-      <c r="A19" t="s">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+    </row>
+    <row r="19" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:27" ht="3.95" customHeight="1">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="22" spans="1:27">
-      <c r="A22" t="s">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+    </row>
+    <row r="22" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:27" ht="3.95" customHeight="1">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-    </row>
-    <row r="25" spans="1:27">
-      <c r="A25" t="s">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:27" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:27" s="6" customFormat="1" ht="3.95" customHeight="1">
-      <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="N26" s="2"/>
-      <c r="AA26" s="2"/>
-    </row>
-    <row r="28" spans="1:27">
-      <c r="A28" t="s">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:27" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="N26" s="1"/>
+      <c r="AA26" s="1"/>
+    </row>
+    <row r="27" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:27" s="6" customFormat="1" ht="3.95" customHeight="1">
-      <c r="F29" s="7"/>
-      <c r="G29" s="9"/>
-      <c r="N29" s="2"/>
-      <c r="AA29" s="2"/>
-    </row>
-    <row r="31" spans="1:27">
-      <c r="A31" t="s">
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+    </row>
+    <row r="29" spans="1:27" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="N29" s="1"/>
+      <c r="AA29" s="1"/>
+    </row>
+    <row r="30" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="1:27" s="6" customFormat="1" ht="3.95" customHeight="1">
-      <c r="F32" s="7"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="N32" s="2"/>
-      <c r="AA32" s="2"/>
-    </row>
-    <row r="34" spans="1:27">
-      <c r="A34" t="s">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:27" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="N32" s="1"/>
+      <c r="AA32" s="1"/>
+    </row>
+    <row r="33" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+    </row>
+    <row r="34" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="1:27" s="6" customFormat="1" ht="3.95" customHeight="1">
-      <c r="F35" s="7"/>
-      <c r="G35" s="9"/>
-      <c r="N35" s="2"/>
-      <c r="AA35" s="2"/>
-    </row>
-    <row r="37" spans="1:27">
-      <c r="A37" t="s">
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="1:27" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="7"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="1"/>
+      <c r="AA35" s="1"/>
+    </row>
+    <row r="36" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-    </row>
-    <row r="38" spans="1:27" s="6" customFormat="1" ht="3.95" customHeight="1">
-      <c r="F38" s="7"/>
-      <c r="G38" s="9"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="2"/>
-      <c r="AA38" s="2"/>
-    </row>
-    <row r="40" spans="1:27">
-      <c r="A40" t="s">
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="1:27" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="7"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="1"/>
+      <c r="AA38" s="1"/>
+    </row>
+    <row r="39" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+    </row>
+    <row r="40" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-    </row>
-    <row r="41" spans="1:27" s="6" customFormat="1" ht="3.95" customHeight="1">
-      <c r="F41" s="7"/>
-      <c r="G41" s="9"/>
-      <c r="N41" s="2"/>
-      <c r="AA41" s="2"/>
-    </row>
-    <row r="43" spans="1:27">
-      <c r="A43" t="s">
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="41" spans="1:27" s="4" customFormat="1" ht="3.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="7"/>
+      <c r="N41" s="1"/>
+      <c r="AA41" s="1"/>
+    </row>
+    <row r="42" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="9"/>
+    </row>
+    <row r="43" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="6"/>
-      <c r="T43" s="6"/>
-      <c r="U43" s="6"/>
-    </row>
-    <row r="44" spans="1:27" s="6" customFormat="1" ht="3.75" customHeight="1">
-      <c r="F44" s="7"/>
-      <c r="G44" s="9"/>
-      <c r="N44" s="2"/>
-      <c r="AA44" s="2"/>
-    </row>
-    <row r="46" spans="1:27">
-      <c r="A46" t="s">
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+    </row>
+    <row r="44" spans="1:27" s="4" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="7"/>
+      <c r="N44" s="1"/>
+      <c r="AA44" s="1"/>
+    </row>
+    <row r="45" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-    </row>
-    <row r="47" spans="1:27" s="6" customFormat="1" ht="3.75" customHeight="1">
-      <c r="F47" s="7"/>
-      <c r="G47" s="9"/>
-      <c r="N47" s="2"/>
-      <c r="AA47" s="2"/>
-    </row>
-    <row r="49" spans="1:27">
-      <c r="A49" t="s">
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="1:27" s="4" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="11"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="7"/>
+      <c r="N47" s="1"/>
+      <c r="AA47" s="1"/>
+    </row>
+    <row r="48" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
+    </row>
+    <row r="49" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-      <c r="X49" s="4"/>
-      <c r="Y49" s="4"/>
-      <c r="Z49" s="4"/>
-    </row>
-    <row r="50" spans="1:27" s="6" customFormat="1" ht="3.75" customHeight="1">
-      <c r="F50" s="7"/>
-      <c r="G50" s="9"/>
-      <c r="N50" s="2"/>
-      <c r="AA50" s="2"/>
-    </row>
-    <row r="52" spans="1:27">
-      <c r="A52" t="s">
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+    </row>
+    <row r="50" spans="1:27" s="4" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="11"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="7"/>
+      <c r="N50" s="1"/>
+      <c r="AA50" s="1"/>
+    </row>
+    <row r="51" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+    </row>
+    <row r="52" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Z52" s="4"/>
-      <c r="AA52" s="4"/>
-    </row>
-    <row r="53" spans="1:27" s="6" customFormat="1" ht="3.75" customHeight="1">
-      <c r="F53" s="7"/>
-      <c r="G53" s="9"/>
-      <c r="N53" s="2"/>
-      <c r="AA53" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+    </row>
+    <row r="53" spans="1:27" s="4" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="5"/>
+      <c r="G53" s="7"/>
+      <c r="N53" s="1"/>
+      <c r="AA53" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>